<commit_message>
more data wrangling and cleaning
</commit_message>
<xml_diff>
--- a/datasets/raw/2016-2022-nsch_crosswalk_cahmi_10-2-23.xlsx
+++ b/datasets/raw/2016-2022-nsch_crosswalk_cahmi_10-2-23.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cloned-directories\HRTL-2016-2022\HRTL-2016-2022\datasets\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\HRTL-2016-2022\datasets\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34CE36F-483F-4CB8-9FA3-130C75881E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71326AAE-5268-4327-84AB-4024F8B4D6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3850" yWindow="2760" windowWidth="16920" windowHeight="10450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18021,6 +18021,45 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -18030,74 +18069,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -18147,62 +18147,62 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20166,39 +20166,39 @@
   <dimension ref="A1:T1053"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="Q393" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="P386" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R394" sqref="R394"/>
+      <selection pane="bottomRight" activeCell="R389" sqref="R389"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.81640625" customWidth="1"/>
-    <col min="15" max="15" width="18.1796875" customWidth="1"/>
-    <col min="16" max="16" width="29.54296875" customWidth="1"/>
-    <col min="17" max="17" width="24.7265625" customWidth="1"/>
-    <col min="18" max="18" width="31.26953125" customWidth="1"/>
-    <col min="19" max="19" width="23.7265625" customWidth="1"/>
+    <col min="14" max="14" width="38.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" customWidth="1"/>
+    <col min="16" max="16" width="29.5703125" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="78.75" customHeight="1">
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -20264,11 +20264,11 @@
       <c r="B4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="185" t="s">
+      <c r="C4" s="237" t="s">
         <v>1460</v>
       </c>
-      <c r="D4" s="186"/>
-      <c r="E4" s="187"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="239"/>
       <c r="F4" s="80" t="s">
         <v>6</v>
       </c>
@@ -20285,20 +20285,20 @@
         <v>9</v>
       </c>
       <c r="M4" s="81"/>
-      <c r="N4" s="239" t="s">
+      <c r="N4" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="240"/>
-      <c r="P4" s="239" t="s">
+      <c r="O4" s="188"/>
+      <c r="P4" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="240"/>
-      <c r="R4" s="239" t="s">
+      <c r="Q4" s="188"/>
+      <c r="R4" s="187" t="s">
         <v>1536</v>
       </c>
-      <c r="S4" s="240"/>
-    </row>
-    <row r="5" spans="2:19" thickBot="1">
+      <c r="S4" s="188"/>
+    </row>
+    <row r="5" spans="2:19" ht="15.75" thickBot="1">
       <c r="B5" s="90"/>
       <c r="C5" s="119" t="s">
         <v>1441</v>
@@ -20352,11 +20352,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:19" hidden="1" thickTop="1">
+    <row r="6" spans="2:19" ht="15.75" hidden="1" thickTop="1">
       <c r="B6" s="91"/>
-      <c r="C6" s="188"/>
-      <c r="D6" s="189"/>
-      <c r="E6" s="190"/>
+      <c r="C6" s="240"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="242"/>
       <c r="F6" s="93" t="s">
         <v>14</v>
       </c>
@@ -20380,15 +20380,15 @@
       <c r="R6" s="141"/>
       <c r="S6" s="142"/>
     </row>
-    <row r="7" spans="2:19" ht="96.5" thickTop="1">
+    <row r="7" spans="2:19" ht="108.75" thickTop="1">
       <c r="B7" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="182" t="s">
+      <c r="C7" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D7" s="183"/>
-      <c r="E7" s="184"/>
+      <c r="D7" s="196"/>
+      <c r="E7" s="197"/>
       <c r="F7" s="10" t="s">
         <v>16</v>
       </c>
@@ -20432,15 +20432,15 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="36">
+    <row r="8" spans="2:19" ht="48">
       <c r="B8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="182" t="s">
+      <c r="C8" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D8" s="183"/>
-      <c r="E8" s="184"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="197"/>
       <c r="F8" s="10" t="s">
         <v>20</v>
       </c>
@@ -20484,15 +20484,15 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="24">
+    <row r="9" spans="2:19" ht="36">
       <c r="B9" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="182" t="s">
+      <c r="C9" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D9" s="183"/>
-      <c r="E9" s="184"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="197"/>
       <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
@@ -20536,15 +20536,15 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="10" spans="2:19" ht="132">
+    <row r="10" spans="2:19" ht="156">
       <c r="B10" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="182" t="s">
+      <c r="C10" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="197"/>
       <c r="F10" s="10"/>
       <c r="G10" s="9"/>
       <c r="H10" s="46"/>
@@ -20580,13 +20580,13 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="130">
+    <row r="11" spans="2:19" ht="127.5">
       <c r="B11" s="85"/>
-      <c r="C11" s="182" t="s">
+      <c r="C11" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D11" s="183"/>
-      <c r="E11" s="184"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="197"/>
       <c r="F11" s="94" t="s">
         <v>1365</v>
       </c>
@@ -20616,13 +20616,13 @@
       </c>
       <c r="S11" s="135"/>
     </row>
-    <row r="12" spans="2:19" ht="26">
+    <row r="12" spans="2:19" ht="25.5">
       <c r="B12" s="85"/>
-      <c r="C12" s="182" t="s">
+      <c r="C12" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D12" s="183"/>
-      <c r="E12" s="184"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="197"/>
       <c r="F12" s="15"/>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
@@ -20650,15 +20650,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:19" ht="39">
+    <row r="13" spans="2:19" ht="38.25">
       <c r="B13" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="182" t="s">
+      <c r="C13" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D13" s="183"/>
-      <c r="E13" s="184"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="197"/>
       <c r="F13" s="10" t="s">
         <v>1477</v>
       </c>
@@ -20702,15 +20702,15 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="14" spans="2:19" ht="14.5">
+    <row r="14" spans="2:19">
       <c r="B14" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="182" t="s">
+      <c r="C14" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D14" s="183"/>
-      <c r="E14" s="184"/>
+      <c r="D14" s="196"/>
+      <c r="E14" s="197"/>
       <c r="F14" s="10" t="s">
         <v>51</v>
       </c>
@@ -20754,15 +20754,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:19" ht="84">
+    <row r="15" spans="2:19" ht="108">
       <c r="B15" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="182" t="s">
+      <c r="C15" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D15" s="183"/>
-      <c r="E15" s="184"/>
+      <c r="D15" s="196"/>
+      <c r="E15" s="197"/>
       <c r="F15" s="60" t="s">
         <v>1353</v>
       </c>
@@ -20807,14 +20807,14 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="24" customHeight="1">
-      <c r="B16" s="195" t="s">
+      <c r="B16" s="224" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="199" t="s">
+      <c r="C16" s="228" t="s">
         <v>1458</v>
       </c>
-      <c r="D16" s="200"/>
-      <c r="E16" s="201"/>
+      <c r="D16" s="229"/>
+      <c r="E16" s="230"/>
       <c r="F16" s="60" t="s">
         <v>1363</v>
       </c>
@@ -20844,11 +20844,11 @@
       </c>
       <c r="S16" s="54"/>
     </row>
-    <row r="17" spans="2:19" ht="14.5" hidden="1">
-      <c r="B17" s="198"/>
-      <c r="C17" s="202"/>
-      <c r="D17" s="203"/>
-      <c r="E17" s="204"/>
+    <row r="17" spans="2:19" hidden="1">
+      <c r="B17" s="227"/>
+      <c r="C17" s="231"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="233"/>
       <c r="F17" s="10" t="s">
         <v>31</v>
       </c>
@@ -20892,11 +20892,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="14.5" hidden="1">
-      <c r="B18" s="198"/>
-      <c r="C18" s="202"/>
-      <c r="D18" s="203"/>
-      <c r="E18" s="204"/>
+    <row r="18" spans="2:19" hidden="1">
+      <c r="B18" s="227"/>
+      <c r="C18" s="231"/>
+      <c r="D18" s="232"/>
+      <c r="E18" s="233"/>
       <c r="F18" s="10" t="s">
         <v>33</v>
       </c>
@@ -20940,11 +20940,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="14.5" hidden="1">
-      <c r="B19" s="198"/>
-      <c r="C19" s="202"/>
-      <c r="D19" s="203"/>
-      <c r="E19" s="204"/>
+    <row r="19" spans="2:19" hidden="1">
+      <c r="B19" s="227"/>
+      <c r="C19" s="231"/>
+      <c r="D19" s="232"/>
+      <c r="E19" s="233"/>
       <c r="F19" s="10" t="s">
         <v>34</v>
       </c>
@@ -20988,11 +20988,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:19" ht="14.5" hidden="1">
-      <c r="B20" s="198"/>
-      <c r="C20" s="202"/>
-      <c r="D20" s="203"/>
-      <c r="E20" s="204"/>
+    <row r="20" spans="2:19" hidden="1">
+      <c r="B20" s="227"/>
+      <c r="C20" s="231"/>
+      <c r="D20" s="232"/>
+      <c r="E20" s="233"/>
       <c r="F20" s="10" t="s">
         <v>35</v>
       </c>
@@ -21036,11 +21036,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:19" ht="14.5" hidden="1">
-      <c r="B21" s="198"/>
-      <c r="C21" s="202"/>
-      <c r="D21" s="203"/>
-      <c r="E21" s="204"/>
+    <row r="21" spans="2:19" hidden="1">
+      <c r="B21" s="227"/>
+      <c r="C21" s="231"/>
+      <c r="D21" s="232"/>
+      <c r="E21" s="233"/>
       <c r="F21" s="10" t="s">
         <v>36</v>
       </c>
@@ -21084,11 +21084,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:19" ht="14.5" hidden="1">
-      <c r="B22" s="198"/>
-      <c r="C22" s="202"/>
-      <c r="D22" s="203"/>
-      <c r="E22" s="204"/>
+    <row r="22" spans="2:19" hidden="1">
+      <c r="B22" s="227"/>
+      <c r="C22" s="231"/>
+      <c r="D22" s="232"/>
+      <c r="E22" s="233"/>
       <c r="F22" s="10" t="s">
         <v>37</v>
       </c>
@@ -21132,11 +21132,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:19" ht="14.5" hidden="1">
-      <c r="B23" s="198"/>
-      <c r="C23" s="202"/>
-      <c r="D23" s="203"/>
-      <c r="E23" s="204"/>
+    <row r="23" spans="2:19" hidden="1">
+      <c r="B23" s="227"/>
+      <c r="C23" s="231"/>
+      <c r="D23" s="232"/>
+      <c r="E23" s="233"/>
       <c r="F23" s="10" t="s">
         <v>38</v>
       </c>
@@ -21180,11 +21180,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:19" ht="14.5" hidden="1">
-      <c r="B24" s="198"/>
-      <c r="C24" s="202"/>
-      <c r="D24" s="203"/>
-      <c r="E24" s="204"/>
+    <row r="24" spans="2:19" hidden="1">
+      <c r="B24" s="227"/>
+      <c r="C24" s="231"/>
+      <c r="D24" s="232"/>
+      <c r="E24" s="233"/>
       <c r="F24" s="10" t="s">
         <v>39</v>
       </c>
@@ -21228,11 +21228,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="14.5" hidden="1">
-      <c r="B25" s="198"/>
-      <c r="C25" s="202"/>
-      <c r="D25" s="203"/>
-      <c r="E25" s="204"/>
+    <row r="25" spans="2:19" hidden="1">
+      <c r="B25" s="227"/>
+      <c r="C25" s="231"/>
+      <c r="D25" s="232"/>
+      <c r="E25" s="233"/>
       <c r="F25" s="10" t="s">
         <v>40</v>
       </c>
@@ -21276,11 +21276,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:19" ht="14.5" hidden="1">
-      <c r="B26" s="198"/>
-      <c r="C26" s="202"/>
-      <c r="D26" s="203"/>
-      <c r="E26" s="204"/>
+    <row r="26" spans="2:19" hidden="1">
+      <c r="B26" s="227"/>
+      <c r="C26" s="231"/>
+      <c r="D26" s="232"/>
+      <c r="E26" s="233"/>
       <c r="F26" s="10" t="s">
         <v>41</v>
       </c>
@@ -21324,11 +21324,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="14.5" hidden="1">
-      <c r="B27" s="198"/>
-      <c r="C27" s="202"/>
-      <c r="D27" s="203"/>
-      <c r="E27" s="204"/>
+    <row r="27" spans="2:19" hidden="1">
+      <c r="B27" s="227"/>
+      <c r="C27" s="231"/>
+      <c r="D27" s="232"/>
+      <c r="E27" s="233"/>
       <c r="F27" s="10" t="s">
         <v>42</v>
       </c>
@@ -21372,11 +21372,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="14.5" hidden="1">
-      <c r="B28" s="198"/>
-      <c r="C28" s="202"/>
-      <c r="D28" s="203"/>
-      <c r="E28" s="204"/>
+    <row r="28" spans="2:19" hidden="1">
+      <c r="B28" s="227"/>
+      <c r="C28" s="231"/>
+      <c r="D28" s="232"/>
+      <c r="E28" s="233"/>
       <c r="F28" s="10" t="s">
         <v>43</v>
       </c>
@@ -21420,11 +21420,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="14.5" hidden="1">
-      <c r="B29" s="198"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="203"/>
-      <c r="E29" s="204"/>
+    <row r="29" spans="2:19" hidden="1">
+      <c r="B29" s="227"/>
+      <c r="C29" s="231"/>
+      <c r="D29" s="232"/>
+      <c r="E29" s="233"/>
       <c r="F29" s="10" t="s">
         <v>44</v>
       </c>
@@ -21468,11 +21468,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="14.5" hidden="1">
-      <c r="B30" s="198"/>
-      <c r="C30" s="202"/>
-      <c r="D30" s="203"/>
-      <c r="E30" s="204"/>
+    <row r="30" spans="2:19" hidden="1">
+      <c r="B30" s="227"/>
+      <c r="C30" s="231"/>
+      <c r="D30" s="232"/>
+      <c r="E30" s="233"/>
       <c r="F30" s="10" t="s">
         <v>45</v>
       </c>
@@ -21516,11 +21516,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="14.5" hidden="1">
-      <c r="B31" s="196"/>
-      <c r="C31" s="205"/>
-      <c r="D31" s="206"/>
-      <c r="E31" s="207"/>
+    <row r="31" spans="2:19" hidden="1">
+      <c r="B31" s="225"/>
+      <c r="C31" s="234"/>
+      <c r="D31" s="235"/>
+      <c r="E31" s="236"/>
       <c r="F31" s="10" t="s">
         <v>46</v>
       </c>
@@ -21568,11 +21568,11 @@
       <c r="B32" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="182" t="s">
+      <c r="C32" s="195" t="s">
         <v>1459</v>
       </c>
-      <c r="D32" s="183"/>
-      <c r="E32" s="184"/>
+      <c r="D32" s="196"/>
+      <c r="E32" s="197"/>
       <c r="F32" s="10" t="s">
         <v>55</v>
       </c>
@@ -21620,11 +21620,11 @@
       <c r="B33" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="182" t="s">
+      <c r="C33" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D33" s="183"/>
-      <c r="E33" s="184"/>
+      <c r="D33" s="196"/>
+      <c r="E33" s="197"/>
       <c r="F33" s="10" t="s">
         <v>58</v>
       </c>
@@ -21668,15 +21668,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="36">
+    <row r="34" spans="1:19" ht="48">
       <c r="B34" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="182" t="s">
+      <c r="C34" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="184"/>
+      <c r="D34" s="196"/>
+      <c r="E34" s="197"/>
       <c r="F34" s="10" t="s">
         <v>60</v>
       </c>
@@ -21720,15 +21720,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="24">
+    <row r="35" spans="1:19" ht="36">
       <c r="B35" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="182" t="s">
+      <c r="C35" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D35" s="183"/>
-      <c r="E35" s="184"/>
+      <c r="D35" s="196"/>
+      <c r="E35" s="197"/>
       <c r="F35" s="10" t="s">
         <v>62</v>
       </c>
@@ -21776,11 +21776,11 @@
       <c r="B36" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="182" t="s">
+      <c r="C36" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D36" s="183"/>
-      <c r="E36" s="184"/>
+      <c r="D36" s="196"/>
+      <c r="E36" s="197"/>
       <c r="F36" s="10" t="s">
         <v>64</v>
       </c>
@@ -21824,15 +21824,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="48">
+    <row r="37" spans="1:19" ht="60">
       <c r="B37" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="182" t="s">
+      <c r="C37" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D37" s="183"/>
-      <c r="E37" s="184"/>
+      <c r="D37" s="196"/>
+      <c r="E37" s="197"/>
       <c r="F37" s="10" t="s">
         <v>66</v>
       </c>
@@ -21876,15 +21876,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="24">
+    <row r="38" spans="1:19" ht="36">
       <c r="B38" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="182" t="s">
+      <c r="C38" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D38" s="183"/>
-      <c r="E38" s="184"/>
+      <c r="D38" s="196"/>
+      <c r="E38" s="197"/>
       <c r="F38" s="10" t="s">
         <v>62</v>
       </c>
@@ -21928,15 +21928,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="36">
+    <row r="39" spans="1:19" ht="48">
       <c r="B39" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="182" t="s">
+      <c r="C39" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D39" s="183"/>
-      <c r="E39" s="184"/>
+      <c r="D39" s="196"/>
+      <c r="E39" s="197"/>
       <c r="F39" s="10" t="s">
         <v>69</v>
       </c>
@@ -21980,15 +21980,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="36">
+    <row r="40" spans="1:19" ht="48">
       <c r="B40" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="182" t="s">
+      <c r="C40" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D40" s="183"/>
-      <c r="E40" s="184"/>
+      <c r="D40" s="196"/>
+      <c r="E40" s="197"/>
       <c r="F40" s="10" t="s">
         <v>71</v>
       </c>
@@ -22032,15 +22032,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="24">
+    <row r="41" spans="1:19" ht="36">
       <c r="B41" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="182" t="s">
+      <c r="C41" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D41" s="183"/>
-      <c r="E41" s="184"/>
+      <c r="D41" s="196"/>
+      <c r="E41" s="197"/>
       <c r="F41" s="10" t="s">
         <v>62</v>
       </c>
@@ -22088,11 +22088,11 @@
       <c r="B42" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="182" t="s">
+      <c r="C42" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="184"/>
+      <c r="D42" s="196"/>
+      <c r="E42" s="197"/>
       <c r="F42" s="10" t="s">
         <v>75</v>
       </c>
@@ -22136,15 +22136,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="24">
+    <row r="43" spans="1:19" ht="36">
       <c r="B43" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="182" t="s">
+      <c r="C43" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D43" s="183"/>
-      <c r="E43" s="184"/>
+      <c r="D43" s="196"/>
+      <c r="E43" s="197"/>
       <c r="F43" s="60" t="s">
         <v>1367</v>
       </c>
@@ -22188,15 +22188,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="24">
+    <row r="44" spans="1:19" ht="36">
       <c r="B44" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="182" t="s">
+      <c r="C44" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="D44" s="196"/>
+      <c r="E44" s="197"/>
       <c r="F44" s="10" t="s">
         <v>62</v>
       </c>
@@ -22240,15 +22240,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="36">
+    <row r="45" spans="1:19" ht="48">
       <c r="B45" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="182" t="s">
+      <c r="C45" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D45" s="183"/>
-      <c r="E45" s="184"/>
+      <c r="D45" s="196"/>
+      <c r="E45" s="197"/>
       <c r="F45" s="10" t="s">
         <v>79</v>
       </c>
@@ -22292,15 +22292,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="36">
+    <row r="46" spans="1:19" ht="48">
       <c r="B46" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="182" t="s">
+      <c r="C46" s="195" t="s">
         <v>1458</v>
       </c>
-      <c r="D46" s="183"/>
-      <c r="E46" s="184"/>
+      <c r="D46" s="196"/>
+      <c r="E46" s="197"/>
       <c r="F46" s="10" t="s">
         <v>81</v>
       </c>
@@ -22344,7 +22344,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14.5" hidden="1">
+    <row r="47" spans="1:19" hidden="1">
       <c r="B47" s="85"/>
       <c r="C47" s="215"/>
       <c r="D47" s="216"/>
@@ -22378,7 +22378,7 @@
       </c>
       <c r="S47" s="14"/>
     </row>
-    <row r="48" spans="1:19" ht="24">
+    <row r="48" spans="1:19" ht="36">
       <c r="A48">
         <v>-1</v>
       </c>
@@ -22437,7 +22437,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="36">
+    <row r="49" spans="1:19" ht="48">
       <c r="A49">
         <v>-1</v>
       </c>
@@ -22640,7 +22640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="24">
+    <row r="53" spans="1:19" ht="36">
       <c r="B53" s="48" t="s">
         <v>109</v>
       </c>
@@ -22960,7 +22960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="48" hidden="1">
+    <row r="59" spans="1:19" ht="60" hidden="1">
       <c r="B59" s="48" t="s">
         <v>1739</v>
       </c>
@@ -23014,7 +23014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="48" hidden="1">
+    <row r="60" spans="1:19" ht="60" hidden="1">
       <c r="B60" s="48" t="s">
         <v>1738</v>
       </c>
@@ -23156,7 +23156,7 @@
       </c>
       <c r="S62" s="42"/>
     </row>
-    <row r="63" spans="1:19" ht="24">
+    <row r="63" spans="1:19" ht="36">
       <c r="B63" s="48" t="s">
         <v>147</v>
       </c>
@@ -23380,7 +23380,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="2:19" ht="14.5">
+    <row r="67" spans="2:19">
       <c r="B67" s="48" t="s">
         <v>155</v>
       </c>
@@ -23432,7 +23432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="2:19" ht="14.5">
+    <row r="68" spans="2:19">
       <c r="B68" s="48" t="s">
         <v>158</v>
       </c>
@@ -23484,7 +23484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="2:19" ht="14.5">
+    <row r="69" spans="2:19">
       <c r="B69" s="48" t="s">
         <v>160</v>
       </c>
@@ -23540,7 +23540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="2:19" ht="14.5">
+    <row r="70" spans="2:19">
       <c r="B70" s="48" t="s">
         <v>162</v>
       </c>
@@ -23596,7 +23596,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="2:19" ht="14.5">
+    <row r="71" spans="2:19">
       <c r="B71" s="48" t="s">
         <v>164</v>
       </c>
@@ -23652,7 +23652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="2:19" ht="14.5" hidden="1">
+    <row r="72" spans="2:19" ht="24" hidden="1">
       <c r="B72" s="86"/>
       <c r="C72" s="96"/>
       <c r="D72" s="97"/>
@@ -23740,7 +23740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="2:19" ht="14.5" hidden="1">
+    <row r="74" spans="2:19" ht="24" hidden="1">
       <c r="B74" s="48" t="s">
         <v>174</v>
       </c>
@@ -23794,7 +23794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="2:19" ht="14.5" hidden="1">
+    <row r="75" spans="2:19" hidden="1">
       <c r="B75" s="48" t="s">
         <v>176</v>
       </c>
@@ -23900,7 +23900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="2:19" ht="14.5">
+    <row r="77" spans="2:19">
       <c r="B77" s="48" t="s">
         <v>168</v>
       </c>
@@ -24158,7 +24158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="2:19" ht="14.5">
+    <row r="82" spans="2:19" ht="24">
       <c r="B82" s="48" t="s">
         <v>186</v>
       </c>
@@ -24214,7 +24214,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="2:19" ht="14.5">
+    <row r="83" spans="2:19">
       <c r="B83" s="48" t="s">
         <v>189</v>
       </c>
@@ -24326,7 +24326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="2:19" ht="14.5">
+    <row r="85" spans="2:19" ht="24">
       <c r="B85" s="48" t="s">
         <v>192</v>
       </c>
@@ -24382,7 +24382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="2:19" ht="14.5">
+    <row r="86" spans="2:19">
       <c r="B86" s="48" t="s">
         <v>193</v>
       </c>
@@ -24494,7 +24494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="2:19" ht="14.5">
+    <row r="88" spans="2:19" ht="24">
       <c r="B88" s="48" t="s">
         <v>196</v>
       </c>
@@ -24550,7 +24550,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="2:19" ht="36.5">
+    <row r="89" spans="2:19" ht="36.75">
       <c r="B89" s="112" t="s">
         <v>1690</v>
       </c>
@@ -24606,7 +24606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="2:19" ht="14.5">
+    <row r="90" spans="2:19" ht="24">
       <c r="B90" s="112" t="s">
         <v>1691</v>
       </c>
@@ -24634,7 +24634,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="2:19" ht="24">
+    <row r="91" spans="2:19" ht="36">
       <c r="B91" s="48" t="s">
         <v>197</v>
       </c>
@@ -24690,7 +24690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="2:19" ht="14.5">
+    <row r="92" spans="2:19">
       <c r="B92" s="48" t="s">
         <v>201</v>
       </c>
@@ -24746,7 +24746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="2:19" ht="14.5">
+    <row r="93" spans="2:19" ht="24">
       <c r="B93" s="48" t="s">
         <v>202</v>
       </c>
@@ -24802,7 +24802,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="94" spans="2:19" ht="24" hidden="1">
+    <row r="94" spans="2:19" ht="36" hidden="1">
       <c r="B94" s="48"/>
       <c r="C94" s="109"/>
       <c r="D94" s="110"/>
@@ -24840,7 +24840,7 @@
       </c>
       <c r="S94" s="42"/>
     </row>
-    <row r="95" spans="2:19" ht="14.5">
+    <row r="95" spans="2:19">
       <c r="B95" s="48" t="s">
         <v>208</v>
       </c>
@@ -24896,7 +24896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="2:19" ht="14.5">
+    <row r="96" spans="2:19">
       <c r="B96" s="48" t="s">
         <v>210</v>
       </c>
@@ -24952,7 +24952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="2:19" ht="36">
+    <row r="97" spans="2:19" ht="48">
       <c r="B97" s="48" t="s">
         <v>1737</v>
       </c>
@@ -25008,7 +25008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="2:19" ht="24">
+    <row r="98" spans="2:19" ht="36">
       <c r="B98" s="48" t="s">
         <v>214</v>
       </c>
@@ -25120,7 +25120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="2:19" ht="14.5">
+    <row r="100" spans="2:19">
       <c r="B100" s="48" t="s">
         <v>221</v>
       </c>
@@ -25176,7 +25176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="2:19" ht="14.5">
+    <row r="101" spans="2:19">
       <c r="B101" s="48" t="s">
         <v>223</v>
       </c>
@@ -25232,7 +25232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="2:19" ht="14.5">
+    <row r="102" spans="2:19">
       <c r="B102" s="48" t="s">
         <v>224</v>
       </c>
@@ -25288,7 +25288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="2:19" ht="14.5">
+    <row r="103" spans="2:19">
       <c r="B103" s="48" t="s">
         <v>225</v>
       </c>
@@ -25400,7 +25400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="2:19" ht="14.5">
+    <row r="105" spans="2:19" ht="24">
       <c r="B105" s="30" t="s">
         <v>228</v>
       </c>
@@ -25456,7 +25456,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="2:19" ht="14.5">
+    <row r="106" spans="2:19">
       <c r="B106" s="48" t="s">
         <v>229</v>
       </c>
@@ -25512,7 +25512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="2:19" ht="14.5">
+    <row r="107" spans="2:19">
       <c r="B107" s="48" t="s">
         <v>231</v>
       </c>
@@ -25554,7 +25554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="2:19" ht="24">
+    <row r="108" spans="2:19" ht="48">
       <c r="B108" s="48" t="s">
         <v>1535</v>
       </c>
@@ -25778,7 +25778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="2:19" ht="24">
+    <row r="112" spans="2:19" ht="36">
       <c r="B112" s="48" t="s">
         <v>1694</v>
       </c>
@@ -25834,7 +25834,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="113" spans="2:19" ht="14.5">
+    <row r="113" spans="2:19">
       <c r="B113" s="48" t="s">
         <v>237</v>
       </c>
@@ -25890,7 +25890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="2:19" ht="14.5">
+    <row r="114" spans="2:19">
       <c r="B114" s="48" t="s">
         <v>239</v>
       </c>
@@ -25946,7 +25946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="2:19" ht="14.5">
+    <row r="115" spans="2:19">
       <c r="B115" s="48" t="s">
         <v>240</v>
       </c>
@@ -26000,7 +26000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="2:19" ht="14.5">
+    <row r="116" spans="2:19">
       <c r="B116" s="48" t="s">
         <v>241</v>
       </c>
@@ -26112,7 +26112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="2:19" ht="14.5">
+    <row r="118" spans="2:19" ht="24">
       <c r="B118" s="48" t="s">
         <v>246</v>
       </c>
@@ -26168,7 +26168,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="2:19" ht="14.5">
+    <row r="119" spans="2:19">
       <c r="B119" s="48" t="s">
         <v>247</v>
       </c>
@@ -26320,7 +26320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="2:19" ht="14.5">
+    <row r="122" spans="2:19" ht="24">
       <c r="B122" s="48" t="s">
         <v>253</v>
       </c>
@@ -26488,7 +26488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="2:19" ht="14.5">
+    <row r="125" spans="2:19" ht="24">
       <c r="B125" s="48" t="s">
         <v>257</v>
       </c>
@@ -26544,7 +26544,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="126" spans="2:19" ht="14.5">
+    <row r="126" spans="2:19">
       <c r="B126" s="48" t="s">
         <v>258</v>
       </c>
@@ -26656,7 +26656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="2:19" ht="14.5">
+    <row r="128" spans="2:19" ht="24">
       <c r="B128" s="48" t="s">
         <v>261</v>
       </c>
@@ -26712,7 +26712,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="2:19" ht="14.5">
+    <row r="129" spans="2:19">
       <c r="B129" s="48" t="s">
         <v>262</v>
       </c>
@@ -26824,7 +26824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="2:19" ht="14.5">
+    <row r="131" spans="2:19" ht="24">
       <c r="B131" s="48" t="s">
         <v>265</v>
       </c>
@@ -26880,7 +26880,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="132" spans="2:19" ht="14.5">
+    <row r="132" spans="2:19">
       <c r="B132" s="48" t="s">
         <v>266</v>
       </c>
@@ -26992,7 +26992,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="2:19" ht="14.5">
+    <row r="134" spans="2:19" ht="24">
       <c r="B134" s="48" t="s">
         <v>269</v>
       </c>
@@ -27048,7 +27048,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="135" spans="2:19" ht="14.5">
+    <row r="135" spans="2:19" ht="24">
       <c r="B135" s="48" t="s">
         <v>270</v>
       </c>
@@ -27104,7 +27104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="2:19" ht="14.5">
+    <row r="136" spans="2:19">
       <c r="B136" s="112" t="s">
         <v>274</v>
       </c>
@@ -27146,7 +27146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="2:19" ht="14.5">
+    <row r="137" spans="2:19" ht="24">
       <c r="B137" s="48"/>
       <c r="C137" s="109" t="s">
         <v>1461</v>
@@ -27192,7 +27192,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="138" spans="2:19" ht="14.5">
+    <row r="138" spans="2:19" ht="24">
       <c r="B138" s="48" t="s">
         <v>277</v>
       </c>
@@ -27304,7 +27304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="2:19" ht="14.5">
+    <row r="140" spans="2:19" ht="24">
       <c r="B140" s="180" t="s">
         <v>1689</v>
       </c>
@@ -27558,7 +27558,7 @@
       </c>
       <c r="S144" s="20"/>
     </row>
-    <row r="145" spans="2:19" ht="14.5">
+    <row r="145" spans="2:19">
       <c r="B145" s="48" t="s">
         <v>291</v>
       </c>
@@ -27670,7 +27670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="2:19" ht="14.5">
+    <row r="147" spans="2:19" ht="24">
       <c r="B147" s="48" t="s">
         <v>294</v>
       </c>
@@ -27726,7 +27726,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="148" spans="2:19" ht="14.5" hidden="1">
+    <row r="148" spans="2:19" hidden="1">
       <c r="B148" s="48" t="s">
         <v>295</v>
       </c>
@@ -27780,7 +27780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="2:19" ht="14.5" hidden="1">
+    <row r="149" spans="2:19" hidden="1">
       <c r="B149" s="48" t="s">
         <v>297</v>
       </c>
@@ -27834,7 +27834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="2:19" ht="24" hidden="1">
+    <row r="150" spans="2:19" ht="36" hidden="1">
       <c r="B150" s="112" t="s">
         <v>298</v>
       </c>
@@ -27888,7 +27888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="2:19" ht="14.5">
+    <row r="151" spans="2:19">
       <c r="B151" s="48" t="s">
         <v>299</v>
       </c>
@@ -28000,7 +28000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="2:19" ht="14.5">
+    <row r="153" spans="2:19" ht="24">
       <c r="B153" s="48" t="s">
         <v>302</v>
       </c>
@@ -28168,7 +28168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="2:19" ht="14.5">
+    <row r="156" spans="2:19" ht="24">
       <c r="B156" s="48" t="s">
         <v>313</v>
       </c>
@@ -28224,7 +28224,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="157" spans="2:19" ht="14.5">
+    <row r="157" spans="2:19">
       <c r="B157" s="48" t="s">
         <v>314</v>
       </c>
@@ -28336,7 +28336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="2:19" ht="14.5">
+    <row r="159" spans="2:19" ht="24">
       <c r="B159" s="48" t="s">
         <v>317</v>
       </c>
@@ -28392,7 +28392,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="160" spans="2:19" ht="14.5">
+    <row r="160" spans="2:19">
       <c r="B160" s="48" t="s">
         <v>318</v>
       </c>
@@ -28504,7 +28504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="2:19" ht="14.5">
+    <row r="162" spans="2:19" ht="24">
       <c r="B162" s="48" t="s">
         <v>322</v>
       </c>
@@ -28560,7 +28560,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="163" spans="2:19" ht="24">
+    <row r="163" spans="2:19" ht="36">
       <c r="B163" s="48" t="s">
         <v>323</v>
       </c>
@@ -28616,7 +28616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="2:19" ht="14.5">
+    <row r="164" spans="2:19">
       <c r="B164" s="48"/>
       <c r="C164" s="109" t="s">
         <v>1461</v>
@@ -28654,7 +28654,7 @@
       <c r="R164" s="58"/>
       <c r="S164" s="56"/>
     </row>
-    <row r="165" spans="2:19" ht="14.5">
+    <row r="165" spans="2:19">
       <c r="B165" s="48" t="s">
         <v>326</v>
       </c>
@@ -28710,7 +28710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="2:19" ht="14.5">
+    <row r="166" spans="2:19">
       <c r="B166" s="48" t="s">
         <v>327</v>
       </c>
@@ -28766,7 +28766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="2:19" ht="60">
+    <row r="167" spans="2:19" ht="84">
       <c r="B167" s="48" t="s">
         <v>328</v>
       </c>
@@ -28878,7 +28878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="2:19" ht="14.5">
+    <row r="169" spans="2:19" ht="24">
       <c r="B169" s="48" t="s">
         <v>333</v>
       </c>
@@ -28990,7 +28990,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="171" spans="2:19" ht="108">
+    <row r="171" spans="2:19" ht="120">
       <c r="B171" s="48" t="s">
         <v>338</v>
       </c>
@@ -29102,7 +29102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="2:19" ht="72">
+    <row r="173" spans="2:19" ht="84">
       <c r="B173" s="48" t="s">
         <v>342</v>
       </c>
@@ -29270,7 +29270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="2:19" ht="14.5">
+    <row r="176" spans="2:19" ht="24">
       <c r="B176" s="48" t="s">
         <v>349</v>
       </c>
@@ -29438,7 +29438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="108">
+    <row r="179" spans="1:19" ht="132">
       <c r="B179" s="48" t="s">
         <v>216</v>
       </c>
@@ -29494,7 +29494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="24">
+    <row r="180" spans="1:19" ht="36">
       <c r="B180" s="48" t="s">
         <v>217</v>
       </c>
@@ -29550,7 +29550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="36">
+    <row r="181" spans="1:19" ht="60">
       <c r="B181" s="48" t="s">
         <v>219</v>
       </c>
@@ -29606,7 +29606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="48">
+    <row r="182" spans="1:19" ht="60">
       <c r="A182">
         <v>-1</v>
       </c>
@@ -29724,7 +29724,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="14.5" hidden="1">
+    <row r="184" spans="1:19" hidden="1">
       <c r="B184" s="85"/>
       <c r="C184" s="209"/>
       <c r="D184" s="210"/>
@@ -29926,7 +29926,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="24">
+    <row r="188" spans="1:19" ht="36">
       <c r="B188" s="48" t="s">
         <v>383</v>
       </c>
@@ -30034,7 +30034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="60">
+    <row r="190" spans="1:19" ht="72">
       <c r="B190" s="48" t="s">
         <v>392</v>
       </c>
@@ -30086,7 +30086,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="72">
+    <row r="191" spans="1:19" ht="84">
       <c r="B191" s="48" t="s">
         <v>399</v>
       </c>
@@ -30138,7 +30138,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="84">
+    <row r="192" spans="1:19" ht="108">
       <c r="B192" s="48" t="s">
         <v>406</v>
       </c>
@@ -30190,7 +30190,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="193" spans="2:19" ht="14.5" hidden="1">
+    <row r="193" spans="2:19" hidden="1">
       <c r="B193" s="181"/>
       <c r="C193" s="209"/>
       <c r="D193" s="210"/>
@@ -30332,7 +30332,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="2:19" ht="104.15" customHeight="1">
+    <row r="196" spans="2:19" ht="104.1" customHeight="1">
       <c r="B196" s="48" t="s">
         <v>419</v>
       </c>
@@ -30444,7 +30444,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="198" spans="2:19" ht="38.5">
+    <row r="198" spans="2:19" ht="48">
       <c r="B198" s="48" t="s">
         <v>212</v>
       </c>
@@ -30500,7 +30500,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="199" spans="2:19" ht="48">
+    <row r="199" spans="2:19" ht="60">
       <c r="B199" s="48" t="s">
         <v>212</v>
       </c>
@@ -30612,7 +30612,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="201" spans="2:19" ht="24">
+    <row r="201" spans="2:19" ht="36">
       <c r="B201" s="48" t="s">
         <v>445</v>
       </c>
@@ -30758,7 +30758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="2:19" ht="14.5" hidden="1">
+    <row r="204" spans="2:19" hidden="1">
       <c r="B204" s="48" t="s">
         <v>1696</v>
       </c>
@@ -30812,7 +30812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="205" spans="2:19" ht="14.5" hidden="1">
+    <row r="205" spans="2:19" hidden="1">
       <c r="B205" s="48" t="s">
         <v>1697</v>
       </c>
@@ -30866,7 +30866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="206" spans="2:19" ht="14.5" hidden="1">
+    <row r="206" spans="2:19" hidden="1">
       <c r="B206" s="48" t="s">
         <v>1698</v>
       </c>
@@ -30920,7 +30920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="2:19" ht="14.5" hidden="1">
+    <row r="207" spans="2:19" hidden="1">
       <c r="B207" s="48" t="s">
         <v>1699</v>
       </c>
@@ -31028,7 +31028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="2:19" ht="14.5" hidden="1">
+    <row r="209" spans="2:19" hidden="1">
       <c r="B209" s="48" t="s">
         <v>1701</v>
       </c>
@@ -31082,7 +31082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="210" spans="2:19" ht="14.5" hidden="1">
+    <row r="210" spans="2:19" ht="24" hidden="1">
       <c r="B210" s="48" t="s">
         <v>1702</v>
       </c>
@@ -31190,7 +31190,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="212" spans="2:19" ht="36" hidden="1">
+    <row r="212" spans="2:19" ht="48" hidden="1">
       <c r="B212" s="48" t="s">
         <v>1704</v>
       </c>
@@ -31684,7 +31684,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="222" spans="2:19" ht="108">
+    <row r="222" spans="2:19" ht="144">
       <c r="B222" s="48" t="s">
         <v>470</v>
       </c>
@@ -31740,7 +31740,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="223" spans="2:19" ht="48">
+    <row r="223" spans="2:19" ht="60">
       <c r="B223" s="48" t="s">
         <v>477</v>
       </c>
@@ -31853,7 +31853,7 @@
       </c>
     </row>
     <row r="225" spans="2:19" ht="24">
-      <c r="B225" s="195" t="s">
+      <c r="B225" s="224" t="s">
         <v>485</v>
       </c>
       <c r="C225" s="218" t="s">
@@ -31877,39 +31877,39 @@
       <c r="I225" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J225" s="226" t="s">
+      <c r="J225" s="189" t="s">
         <v>488</v>
       </c>
-      <c r="K225" s="228" t="s">
-        <v>17</v>
-      </c>
-      <c r="L225" s="230" t="s">
+      <c r="K225" s="191" t="s">
+        <v>17</v>
+      </c>
+      <c r="L225" s="204" t="s">
         <v>489</v>
       </c>
-      <c r="M225" s="228" t="s">
-        <v>17</v>
-      </c>
-      <c r="N225" s="226" t="s">
+      <c r="M225" s="191" t="s">
+        <v>17</v>
+      </c>
+      <c r="N225" s="189" t="s">
         <v>1485</v>
       </c>
-      <c r="O225" s="228" t="s">
-        <v>17</v>
-      </c>
-      <c r="P225" s="224" t="s">
+      <c r="O225" s="191" t="s">
+        <v>17</v>
+      </c>
+      <c r="P225" s="200" t="s">
         <v>47</v>
       </c>
-      <c r="Q225" s="241" t="s">
-        <v>15</v>
-      </c>
-      <c r="R225" s="235" t="s">
-        <v>15</v>
-      </c>
-      <c r="S225" s="237" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="226" spans="2:19" ht="24" hidden="1">
-      <c r="B226" s="196"/>
+      <c r="Q225" s="193" t="s">
+        <v>15</v>
+      </c>
+      <c r="R225" s="183" t="s">
+        <v>15</v>
+      </c>
+      <c r="S225" s="185" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="2:19" ht="36" hidden="1">
+      <c r="B226" s="225"/>
       <c r="C226" s="219"/>
       <c r="D226" s="221"/>
       <c r="E226" s="223"/>
@@ -31925,16 +31925,16 @@
       <c r="I226" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J226" s="227"/>
-      <c r="K226" s="229"/>
-      <c r="L226" s="231"/>
-      <c r="M226" s="229"/>
-      <c r="N226" s="192"/>
-      <c r="O226" s="194"/>
-      <c r="P226" s="225"/>
-      <c r="Q226" s="242"/>
-      <c r="R226" s="236"/>
-      <c r="S226" s="238"/>
+      <c r="J226" s="202"/>
+      <c r="K226" s="203"/>
+      <c r="L226" s="205"/>
+      <c r="M226" s="203"/>
+      <c r="N226" s="190"/>
+      <c r="O226" s="192"/>
+      <c r="P226" s="201"/>
+      <c r="Q226" s="194"/>
+      <c r="R226" s="184"/>
+      <c r="S226" s="186"/>
     </row>
     <row r="227" spans="2:19" ht="24" hidden="1">
       <c r="B227" s="87"/>
@@ -32030,7 +32030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="2:19" ht="14.5">
+    <row r="229" spans="2:19">
       <c r="B229" s="48" t="s">
         <v>497</v>
       </c>
@@ -32086,7 +32086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="2:19" ht="14.5">
+    <row r="230" spans="2:19">
       <c r="B230" s="48" t="s">
         <v>499</v>
       </c>
@@ -32142,7 +32142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="2:19" ht="14.5">
+    <row r="231" spans="2:19">
       <c r="B231" s="48" t="s">
         <v>502</v>
       </c>
@@ -32198,7 +32198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="2:19" ht="14.5">
+    <row r="232" spans="2:19" ht="24">
       <c r="B232" s="48" t="s">
         <v>504</v>
       </c>
@@ -32254,7 +32254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="2:19" ht="86.5" customHeight="1">
+    <row r="233" spans="2:19" ht="86.45" customHeight="1">
       <c r="B233" s="136" t="s">
         <v>1516</v>
       </c>
@@ -32306,7 +32306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="2:19" ht="96" hidden="1">
+    <row r="234" spans="2:19" ht="108" hidden="1">
       <c r="B234" s="136" t="s">
         <v>1516</v>
       </c>
@@ -32360,7 +32360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="2:19" ht="84">
+    <row r="235" spans="2:19" ht="96">
       <c r="B235" s="136" t="s">
         <v>1517</v>
       </c>
@@ -32416,7 +32416,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="236" spans="2:19" ht="36">
+    <row r="236" spans="2:19" ht="48">
       <c r="B236" s="136" t="s">
         <v>1518</v>
       </c>
@@ -32546,7 +32546,7 @@
       </c>
       <c r="S238" s="42"/>
     </row>
-    <row r="239" spans="2:19" ht="14.5">
+    <row r="239" spans="2:19">
       <c r="B239" s="136" t="s">
         <v>1519</v>
       </c>
@@ -32602,7 +32602,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="240" spans="2:19" ht="14.5">
+    <row r="240" spans="2:19" ht="24">
       <c r="B240" s="136" t="s">
         <v>1520</v>
       </c>
@@ -32658,7 +32658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="241" spans="2:19" ht="24">
+    <row r="241" spans="2:19" ht="48">
       <c r="B241" s="136" t="s">
         <v>1521</v>
       </c>
@@ -32714,7 +32714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="242" spans="2:19" ht="14.5">
+    <row r="242" spans="2:19">
       <c r="B242" s="136" t="s">
         <v>1523</v>
       </c>
@@ -32770,7 +32770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="243" spans="2:19" ht="60">
+    <row r="243" spans="2:19" ht="72">
       <c r="B243" s="137" t="s">
         <v>1736</v>
       </c>
@@ -32826,7 +32826,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="244" spans="2:19" ht="60">
+    <row r="244" spans="2:19" ht="72">
       <c r="B244" s="129" t="s">
         <v>510</v>
       </c>
@@ -32882,7 +32882,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="245" spans="2:19" ht="36">
+    <row r="245" spans="2:19" ht="48">
       <c r="B245" s="48" t="s">
         <v>514</v>
       </c>
@@ -32924,7 +32924,7 @@
       </c>
       <c r="S245" s="42"/>
     </row>
-    <row r="246" spans="2:19" ht="14.5">
+    <row r="246" spans="2:19">
       <c r="B246" s="48" t="s">
         <v>515</v>
       </c>
@@ -32980,7 +32980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="247" spans="2:19" ht="14.5">
+    <row r="247" spans="2:19">
       <c r="B247" s="48" t="s">
         <v>517</v>
       </c>
@@ -33092,7 +33092,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="249" spans="2:19" ht="14.5">
+    <row r="249" spans="2:19">
       <c r="B249" s="48" t="s">
         <v>521</v>
       </c>
@@ -33148,7 +33148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="250" spans="2:19" ht="14.5">
+    <row r="250" spans="2:19">
       <c r="B250" s="48" t="s">
         <v>523</v>
       </c>
@@ -33204,7 +33204,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="251" spans="2:19" ht="14.5">
+    <row r="251" spans="2:19" ht="24">
       <c r="B251" s="48" t="s">
         <v>525</v>
       </c>
@@ -33260,7 +33260,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="252" spans="2:19" ht="14.5">
+    <row r="252" spans="2:19">
       <c r="B252" s="48" t="s">
         <v>527</v>
       </c>
@@ -33316,7 +33316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="253" spans="2:19" ht="72">
+    <row r="253" spans="2:19" ht="84">
       <c r="B253" s="48" t="s">
         <v>529</v>
       </c>
@@ -33372,7 +33372,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="254" spans="2:19" ht="48">
+    <row r="254" spans="2:19" ht="60">
       <c r="B254" s="48" t="s">
         <v>537</v>
       </c>
@@ -33428,7 +33428,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="255" spans="2:19" ht="48">
+    <row r="255" spans="2:19" ht="60">
       <c r="B255" s="48" t="s">
         <v>543</v>
       </c>
@@ -33484,7 +33484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="256" spans="2:19" ht="72">
+    <row r="256" spans="2:19" ht="84">
       <c r="B256" s="48" t="s">
         <v>546</v>
       </c>
@@ -33540,7 +33540,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="257" spans="2:19" ht="48">
+    <row r="257" spans="2:19" ht="60">
       <c r="B257" s="48" t="s">
         <v>554</v>
       </c>
@@ -33596,7 +33596,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="258" spans="2:19" ht="96">
+    <row r="258" spans="2:19" ht="120">
       <c r="B258" s="48" t="s">
         <v>558</v>
       </c>
@@ -33652,7 +33652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="259" spans="2:19" ht="72">
+    <row r="259" spans="2:19" ht="84">
       <c r="B259" s="48" t="s">
         <v>565</v>
       </c>
@@ -33748,7 +33748,7 @@
       </c>
       <c r="S260" s="54"/>
     </row>
-    <row r="261" spans="2:19" ht="14.5">
+    <row r="261" spans="2:19">
       <c r="B261" s="48" t="s">
         <v>572</v>
       </c>
@@ -33804,7 +33804,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="262" spans="2:19" ht="14.5">
+    <row r="262" spans="2:19">
       <c r="B262" s="48" t="s">
         <v>574</v>
       </c>
@@ -33860,7 +33860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="263" spans="2:19" ht="14.5">
+    <row r="263" spans="2:19">
       <c r="B263" s="48" t="s">
         <v>576</v>
       </c>
@@ -33916,7 +33916,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="264" spans="2:19" ht="14.5">
+    <row r="264" spans="2:19">
       <c r="B264" s="48" t="s">
         <v>578</v>
       </c>
@@ -33972,7 +33972,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="265" spans="2:19" ht="14.5">
+    <row r="265" spans="2:19">
       <c r="B265" s="48" t="s">
         <v>580</v>
       </c>
@@ -34028,7 +34028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="266" spans="2:19" ht="14.5">
+    <row r="266" spans="2:19" ht="24">
       <c r="B266" s="48" t="s">
         <v>582</v>
       </c>
@@ -34124,7 +34124,7 @@
       </c>
       <c r="S267" s="42"/>
     </row>
-    <row r="268" spans="2:19" ht="14.5">
+    <row r="268" spans="2:19" ht="24">
       <c r="B268" s="48" t="s">
         <v>587</v>
       </c>
@@ -34236,7 +34236,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="270" spans="2:19" ht="24">
+    <row r="270" spans="2:19" ht="36">
       <c r="B270" s="48" t="s">
         <v>593</v>
       </c>
@@ -34404,7 +34404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="273" spans="2:19" ht="14.5">
+    <row r="273" spans="2:19">
       <c r="B273" s="48" t="s">
         <v>604</v>
       </c>
@@ -34628,7 +34628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="277" spans="2:19" ht="60">
+    <row r="277" spans="2:19" ht="72">
       <c r="B277" s="48" t="s">
         <v>618</v>
       </c>
@@ -34852,7 +34852,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="281" spans="2:19" ht="24">
+    <row r="281" spans="2:19" ht="36">
       <c r="B281" s="48" t="s">
         <v>634</v>
       </c>
@@ -34964,7 +34964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="283" spans="2:19" ht="60">
+    <row r="283" spans="2:19" ht="72">
       <c r="B283" s="112" t="s">
         <v>1705</v>
       </c>
@@ -35020,7 +35020,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="284" spans="2:19" ht="24">
+    <row r="284" spans="2:19" ht="36">
       <c r="B284" s="112" t="s">
         <v>1706</v>
       </c>
@@ -35110,7 +35110,7 @@
       </c>
       <c r="S285" s="14"/>
     </row>
-    <row r="286" spans="2:19" ht="96">
+    <row r="286" spans="2:19" ht="108">
       <c r="B286" s="48" t="s">
         <v>644</v>
       </c>
@@ -35222,7 +35222,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="288" spans="2:19" ht="48">
+    <row r="288" spans="2:19" ht="60">
       <c r="B288" s="48" t="s">
         <v>654</v>
       </c>
@@ -35278,7 +35278,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="289" spans="2:19" ht="60" hidden="1">
+    <row r="289" spans="2:19" ht="72" hidden="1">
       <c r="B289" s="48"/>
       <c r="C289" s="109"/>
       <c r="D289" s="110"/>
@@ -35626,7 +35626,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="296" spans="2:19" ht="60">
+    <row r="296" spans="2:19" ht="72">
       <c r="B296" s="48" t="s">
         <v>671</v>
       </c>
@@ -35778,7 +35778,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="299" spans="2:19" ht="36">
+    <row r="299" spans="2:19" ht="48">
       <c r="B299" s="48" t="s">
         <v>679</v>
       </c>
@@ -35834,7 +35834,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="300" spans="2:19" ht="36">
+    <row r="300" spans="2:19" ht="48">
       <c r="B300" s="48" t="s">
         <v>681</v>
       </c>
@@ -35890,7 +35890,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="301" spans="2:19" ht="48">
+    <row r="301" spans="2:19" ht="60">
       <c r="B301" s="48" t="s">
         <v>683</v>
       </c>
@@ -36002,7 +36002,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="303" spans="2:19" ht="48">
+    <row r="303" spans="2:19" ht="60">
       <c r="B303" s="48" t="s">
         <v>690</v>
       </c>
@@ -36058,7 +36058,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="304" spans="2:19" ht="48">
+    <row r="304" spans="2:19" ht="60">
       <c r="B304" s="48" t="s">
         <v>693</v>
       </c>
@@ -36114,7 +36114,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="305" spans="2:19" ht="48">
+    <row r="305" spans="2:19" ht="60">
       <c r="B305" s="48" t="s">
         <v>698</v>
       </c>
@@ -36170,7 +36170,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="306" spans="2:19" ht="48">
+    <row r="306" spans="2:19" ht="60">
       <c r="B306" s="48" t="s">
         <v>701</v>
       </c>
@@ -36226,7 +36226,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="307" spans="2:19" ht="24" hidden="1">
+    <row r="307" spans="2:19" ht="36" hidden="1">
       <c r="B307" s="48" t="s">
         <v>705</v>
       </c>
@@ -36330,7 +36330,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="309" spans="2:19" ht="24" hidden="1">
+    <row r="309" spans="2:19" ht="36" hidden="1">
       <c r="B309" s="48"/>
       <c r="C309" s="96"/>
       <c r="D309" s="97"/>
@@ -36364,7 +36364,7 @@
       </c>
       <c r="S309" s="42"/>
     </row>
-    <row r="310" spans="2:19" ht="36" hidden="1">
+    <row r="310" spans="2:19" ht="48" hidden="1">
       <c r="B310" s="48" t="s">
         <v>712</v>
       </c>
@@ -36416,7 +36416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="2:19" ht="48" hidden="1">
+    <row r="311" spans="2:19" ht="60" hidden="1">
       <c r="B311" s="48" t="s">
         <v>715</v>
       </c>
@@ -36520,7 +36520,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="313" spans="2:19" ht="48" hidden="1">
+    <row r="313" spans="2:19" ht="60" hidden="1">
       <c r="B313" s="48" t="s">
         <v>721</v>
       </c>
@@ -36572,7 +36572,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="314" spans="2:19" ht="48" hidden="1">
+    <row r="314" spans="2:19" ht="60" hidden="1">
       <c r="B314" s="48" t="s">
         <v>724</v>
       </c>
@@ -36624,7 +36624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="315" spans="2:19" ht="48" hidden="1">
+    <row r="315" spans="2:19" ht="60" hidden="1">
       <c r="B315" s="48" t="s">
         <v>727</v>
       </c>
@@ -36780,7 +36780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="318" spans="2:19" ht="14.5" hidden="1">
+    <row r="318" spans="2:19" hidden="1">
       <c r="B318" s="48" t="s">
         <v>738</v>
       </c>
@@ -36832,7 +36832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="2:19" ht="36" hidden="1">
+    <row r="319" spans="2:19" ht="48" hidden="1">
       <c r="B319" s="48" t="s">
         <v>740</v>
       </c>
@@ -37022,7 +37022,7 @@
       </c>
       <c r="S322" s="14"/>
     </row>
-    <row r="323" spans="2:19" ht="48">
+    <row r="323" spans="2:19" ht="60">
       <c r="B323" s="48" t="s">
         <v>749</v>
       </c>
@@ -37078,7 +37078,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="324" spans="2:19" ht="48">
+    <row r="324" spans="2:19" ht="60">
       <c r="B324" s="48"/>
       <c r="C324" s="109" t="s">
         <v>1461</v>
@@ -37118,7 +37118,7 @@
       </c>
       <c r="S324" s="42"/>
     </row>
-    <row r="325" spans="2:19" ht="14.5">
+    <row r="325" spans="2:19" ht="24">
       <c r="B325" s="48" t="s">
         <v>755</v>
       </c>
@@ -37174,7 +37174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="326" spans="2:19" ht="14.5">
+    <row r="326" spans="2:19" ht="24">
       <c r="B326" s="48" t="s">
         <v>757</v>
       </c>
@@ -37342,7 +37342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="329" spans="2:19" ht="24">
+    <row r="329" spans="2:19" ht="36">
       <c r="B329" s="48" t="s">
         <v>763</v>
       </c>
@@ -37454,7 +37454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="2:19" ht="14.5">
+    <row r="331" spans="2:19" ht="24">
       <c r="B331" s="48" t="s">
         <v>767</v>
       </c>
@@ -37718,7 +37718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="336" spans="2:19" ht="36">
+    <row r="336" spans="2:19" ht="48">
       <c r="B336" s="48" t="s">
         <v>776</v>
       </c>
@@ -37774,7 +37774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="337" spans="2:19" ht="14.5">
+    <row r="337" spans="2:19" ht="24">
       <c r="B337" s="48" t="s">
         <v>778</v>
       </c>
@@ -37830,7 +37830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="338" spans="2:19" ht="14.5">
+    <row r="338" spans="2:19">
       <c r="B338" s="48" t="s">
         <v>780</v>
       </c>
@@ -37886,7 +37886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="339" spans="2:19" ht="14.5">
+    <row r="339" spans="2:19" ht="24">
       <c r="B339" s="48" t="s">
         <v>783</v>
       </c>
@@ -37942,7 +37942,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="340" spans="2:19" ht="36">
+    <row r="340" spans="2:19" ht="48">
       <c r="B340" s="48" t="s">
         <v>785</v>
       </c>
@@ -38054,7 +38054,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="342" spans="2:19" ht="60">
+    <row r="342" spans="2:19" ht="72">
       <c r="B342" s="48" t="s">
         <v>790</v>
       </c>
@@ -38110,7 +38110,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="343" spans="2:19" ht="26" hidden="1">
+    <row r="343" spans="2:19" ht="25.5" hidden="1">
       <c r="B343" s="85"/>
       <c r="C343" s="209"/>
       <c r="D343" s="210"/>
@@ -38144,7 +38144,7 @@
       </c>
       <c r="S343" s="14"/>
     </row>
-    <row r="344" spans="2:19" ht="108">
+    <row r="344" spans="2:19" ht="132">
       <c r="B344" s="48" t="s">
         <v>795</v>
       </c>
@@ -38256,7 +38256,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="346" spans="2:19" ht="36">
+    <row r="346" spans="2:19" ht="48">
       <c r="B346" s="48" t="s">
         <v>806</v>
       </c>
@@ -38402,7 +38402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="349" spans="2:19" ht="24">
+    <row r="349" spans="2:19" ht="36">
       <c r="B349" s="48" t="s">
         <v>813</v>
       </c>
@@ -38514,7 +38514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="351" spans="2:19" ht="108">
+    <row r="351" spans="2:19" ht="120">
       <c r="B351" s="48" t="s">
         <v>817</v>
       </c>
@@ -38570,7 +38570,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="352" spans="2:19" ht="120">
+    <row r="352" spans="2:19" ht="132">
       <c r="B352" s="48" t="s">
         <v>828</v>
       </c>
@@ -38742,7 +38742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="356" spans="2:19" ht="14.5">
+    <row r="356" spans="2:19" ht="24">
       <c r="B356" s="48" t="s">
         <v>836</v>
       </c>
@@ -38898,7 +38898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="359" spans="2:19" ht="14.5">
+    <row r="359" spans="2:19" ht="24">
       <c r="B359" s="48" t="s">
         <v>842</v>
       </c>
@@ -39054,7 +39054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="362" spans="2:19" ht="24">
+    <row r="362" spans="2:19" ht="36">
       <c r="B362" s="48" t="s">
         <v>848</v>
       </c>
@@ -39106,7 +39106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="363" spans="2:19" ht="14.5">
+    <row r="363" spans="2:19" ht="24">
       <c r="B363" s="48" t="s">
         <v>850</v>
       </c>
@@ -39158,7 +39158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="364" spans="2:19" ht="24">
+    <row r="364" spans="2:19" ht="36">
       <c r="B364" s="48" t="s">
         <v>852</v>
       </c>
@@ -39262,7 +39262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="366" spans="2:19" ht="14.5">
+    <row r="366" spans="2:19">
       <c r="B366" s="48"/>
       <c r="C366" s="109" t="s">
         <v>1461</v>
@@ -39464,7 +39464,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="48">
+    <row r="370" spans="1:20" ht="60">
       <c r="A370">
         <v>-1</v>
       </c>
@@ -39520,7 +39520,7 @@
       </c>
       <c r="T370" s="140"/>
     </row>
-    <row r="371" spans="1:20" ht="36">
+    <row r="371" spans="1:20" ht="48">
       <c r="A371">
         <v>-1</v>
       </c>
@@ -39552,7 +39552,7 @@
       </c>
       <c r="T371" s="140"/>
     </row>
-    <row r="372" spans="1:20" ht="36">
+    <row r="372" spans="1:20" ht="48">
       <c r="A372">
         <v>-1</v>
       </c>
@@ -39607,7 +39607,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="36">
+    <row r="373" spans="1:20" ht="48">
       <c r="A373">
         <v>-1</v>
       </c>
@@ -39827,7 +39827,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="48">
+    <row r="377" spans="1:20" ht="60">
       <c r="A377">
         <v>-1</v>
       </c>
@@ -39994,7 +39994,7 @@
     </row>
     <row r="380" spans="1:20" ht="36">
       <c r="A380">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B380" s="48" t="s">
         <v>1732</v>
@@ -40047,7 +40047,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="36">
+    <row r="381" spans="1:20" ht="48">
       <c r="A381">
         <v>1</v>
       </c>
@@ -40153,7 +40153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="36">
+    <row r="383" spans="1:20" ht="48">
       <c r="A383">
         <v>1</v>
       </c>
@@ -40208,7 +40208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="1:20" ht="36">
+    <row r="384" spans="1:20" ht="48">
       <c r="A384">
         <v>1</v>
       </c>
@@ -40263,7 +40263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="48">
+    <row r="385" spans="1:19" ht="60">
       <c r="A385">
         <v>-1</v>
       </c>
@@ -40318,9 +40318,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="24">
+    <row r="386" spans="1:19" ht="36">
       <c r="A386">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B386" s="48" t="s">
         <v>1712</v>
@@ -40373,9 +40373,9 @@
         <v>882</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="36">
+    <row r="387" spans="1:19" ht="48">
       <c r="A387">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B387" s="48" t="s">
         <v>1733</v>
@@ -40428,7 +40428,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="36">
+    <row r="388" spans="1:19" ht="48">
       <c r="A388">
         <v>-1</v>
       </c>
@@ -40483,7 +40483,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="36">
+    <row r="389" spans="1:19" ht="48">
       <c r="A389">
         <v>1</v>
       </c>
@@ -40538,7 +40538,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="36">
+    <row r="390" spans="1:19" ht="48">
       <c r="A390">
         <v>-1</v>
       </c>
@@ -40593,7 +40593,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="36">
+    <row r="391" spans="1:19" ht="48">
       <c r="A391">
         <v>-1</v>
       </c>
@@ -40648,9 +40648,9 @@
         <v>882</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="36">
+    <row r="392" spans="1:19" ht="48">
       <c r="A392">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B392" s="48" t="s">
         <v>1735</v>
@@ -40703,7 +40703,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="24">
+    <row r="393" spans="1:19" ht="36">
       <c r="A393">
         <v>-1</v>
       </c>
@@ -40758,7 +40758,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="394" spans="1:19" ht="24">
+    <row r="394" spans="1:19" ht="36">
       <c r="A394">
         <v>-1</v>
       </c>
@@ -40813,7 +40813,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="395" spans="1:19" ht="24">
+    <row r="395" spans="1:19" ht="36">
       <c r="A395">
         <v>0</v>
       </c>
@@ -40966,7 +40966,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="36">
+    <row r="398" spans="1:19" ht="48">
       <c r="A398">
         <v>-1</v>
       </c>
@@ -41076,7 +41076,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="60">
+    <row r="400" spans="1:19" ht="72">
       <c r="A400">
         <v>1</v>
       </c>
@@ -41135,7 +41135,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="36">
+    <row r="401" spans="1:19" ht="48">
       <c r="A401">
         <v>1</v>
       </c>
@@ -41190,7 +41190,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="14.5" hidden="1">
+    <row r="402" spans="1:19" hidden="1">
       <c r="B402" s="48"/>
       <c r="C402" s="109"/>
       <c r="D402" s="97"/>
@@ -41395,7 +41395,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="96">
+    <row r="407" spans="1:19" ht="108">
       <c r="B407" s="48" t="s">
         <v>944</v>
       </c>
@@ -41447,7 +41447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="60" hidden="1">
+    <row r="408" spans="1:19" ht="72" hidden="1">
       <c r="B408" s="48" t="s">
         <v>947</v>
       </c>
@@ -41501,7 +41501,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="48" hidden="1">
+    <row r="409" spans="1:19" ht="60" hidden="1">
       <c r="B409" s="48" t="s">
         <v>951</v>
       </c>
@@ -41555,7 +41555,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="60" hidden="1">
+    <row r="410" spans="1:19" ht="72" hidden="1">
       <c r="B410" s="48" t="s">
         <v>1721</v>
       </c>
@@ -41701,7 +41701,7 @@
       </c>
       <c r="S412" s="42"/>
     </row>
-    <row r="413" spans="1:19" ht="24" hidden="1">
+    <row r="413" spans="1:19" ht="36" hidden="1">
       <c r="B413" s="48" t="s">
         <v>958</v>
       </c>
@@ -41971,7 +41971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="418" spans="2:19" ht="36" hidden="1">
+    <row r="418" spans="2:19" ht="48" hidden="1">
       <c r="B418" s="48" t="s">
         <v>971</v>
       </c>
@@ -42025,7 +42025,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="419" spans="2:19" ht="48" hidden="1">
+    <row r="419" spans="2:19" ht="60" hidden="1">
       <c r="B419" s="48" t="s">
         <v>974</v>
       </c>
@@ -42079,7 +42079,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="420" spans="2:19" ht="72" hidden="1">
+    <row r="420" spans="2:19" ht="84" hidden="1">
       <c r="B420" s="48" t="s">
         <v>977</v>
       </c>
@@ -42125,7 +42125,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="421" spans="2:19" ht="72" hidden="1">
+    <row r="421" spans="2:19" ht="84" hidden="1">
       <c r="B421" s="48" t="s">
         <v>979</v>
       </c>
@@ -42171,7 +42171,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="422" spans="2:19" ht="14.5" hidden="1">
+    <row r="422" spans="2:19" hidden="1">
       <c r="B422" s="48"/>
       <c r="C422" s="96"/>
       <c r="D422" s="97"/>
@@ -42205,7 +42205,7 @@
       </c>
       <c r="S422" s="42"/>
     </row>
-    <row r="423" spans="2:19" ht="26" hidden="1">
+    <row r="423" spans="2:19" ht="25.5" hidden="1">
       <c r="B423" s="48" t="s">
         <v>109</v>
       </c>
@@ -42481,7 +42481,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="429" spans="2:19" ht="14.5" hidden="1">
+    <row r="429" spans="2:19" hidden="1">
       <c r="B429" s="88"/>
       <c r="C429" s="212"/>
       <c r="D429" s="213"/>
@@ -42515,7 +42515,7 @@
       </c>
       <c r="S429" s="14"/>
     </row>
-    <row r="430" spans="2:19" ht="14.5">
+    <row r="430" spans="2:19" ht="24">
       <c r="B430" s="48" t="s">
         <v>985</v>
       </c>
@@ -42571,7 +42571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="431" spans="2:19" ht="24">
+    <row r="431" spans="2:19" ht="36">
       <c r="B431" s="48" t="s">
         <v>987</v>
       </c>
@@ -42627,7 +42627,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="432" spans="2:19" ht="24">
+    <row r="432" spans="2:19" ht="36">
       <c r="B432" s="48" t="s">
         <v>990</v>
       </c>
@@ -42683,7 +42683,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="433" spans="2:19" ht="24">
+    <row r="433" spans="2:19" ht="36">
       <c r="B433" s="48" t="s">
         <v>994</v>
       </c>
@@ -42739,7 +42739,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="434" spans="2:19" ht="48">
+    <row r="434" spans="2:19" ht="60">
       <c r="B434" s="48" t="s">
         <v>996</v>
       </c>
@@ -42791,7 +42791,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="435" spans="2:19" ht="48" hidden="1">
+    <row r="435" spans="2:19" ht="60" hidden="1">
       <c r="B435" s="48" t="s">
         <v>999</v>
       </c>
@@ -42845,7 +42845,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="436" spans="2:19" ht="48">
+    <row r="436" spans="2:19" ht="60">
       <c r="B436" s="48" t="s">
         <v>1004</v>
       </c>
@@ -42897,7 +42897,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="437" spans="2:19" ht="60">
+    <row r="437" spans="2:19" ht="72">
       <c r="B437" s="136" t="s">
         <v>1528</v>
       </c>
@@ -42949,7 +42949,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="438" spans="2:19" ht="60">
+    <row r="438" spans="2:19" ht="72">
       <c r="B438" s="136" t="s">
         <v>1527</v>
       </c>
@@ -43001,7 +43001,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="439" spans="2:19" ht="60">
+    <row r="439" spans="2:19" ht="72">
       <c r="B439" s="136" t="s">
         <v>1526</v>
       </c>
@@ -43105,7 +43105,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="441" spans="2:19" ht="108">
+    <row r="441" spans="2:19" ht="120">
       <c r="B441" s="136" t="s">
         <v>1524</v>
       </c>
@@ -43182,34 +43182,34 @@
       <c r="I442" s="42" t="s">
         <v>1007</v>
       </c>
-      <c r="J442" s="232" t="s">
+      <c r="J442" s="206" t="s">
         <v>1008</v>
       </c>
-      <c r="K442" s="228" t="s">
+      <c r="K442" s="191" t="s">
         <v>1009</v>
       </c>
-      <c r="L442" s="226" t="s">
+      <c r="L442" s="189" t="s">
         <v>1008</v>
       </c>
-      <c r="M442" s="228" t="s">
+      <c r="M442" s="191" t="s">
         <v>1009</v>
       </c>
-      <c r="N442" s="191" t="s">
+      <c r="N442" s="199" t="s">
         <v>1010</v>
       </c>
-      <c r="O442" s="193" t="s">
+      <c r="O442" s="198" t="s">
         <v>1009</v>
       </c>
-      <c r="P442" s="191" t="s">
+      <c r="P442" s="199" t="s">
         <v>1451</v>
       </c>
-      <c r="Q442" s="193" t="s">
+      <c r="Q442" s="198" t="s">
         <v>1009</v>
       </c>
-      <c r="R442" s="191" t="s">
+      <c r="R442" s="199" t="s">
         <v>1451</v>
       </c>
-      <c r="S442" s="193" t="s">
+      <c r="S442" s="198" t="s">
         <v>1009</v>
       </c>
     </row>
@@ -43238,16 +43238,16 @@
       <c r="I443" s="42" t="s">
         <v>1007</v>
       </c>
-      <c r="J443" s="233"/>
-      <c r="K443" s="229"/>
-      <c r="L443" s="227"/>
-      <c r="M443" s="229"/>
-      <c r="N443" s="192"/>
-      <c r="O443" s="194"/>
-      <c r="P443" s="192"/>
-      <c r="Q443" s="194"/>
-      <c r="R443" s="192"/>
-      <c r="S443" s="194"/>
+      <c r="J443" s="207"/>
+      <c r="K443" s="203"/>
+      <c r="L443" s="202"/>
+      <c r="M443" s="203"/>
+      <c r="N443" s="190"/>
+      <c r="O443" s="192"/>
+      <c r="P443" s="190"/>
+      <c r="Q443" s="192"/>
+      <c r="R443" s="190"/>
+      <c r="S443" s="192"/>
     </row>
     <row r="444" spans="2:19" ht="36" hidden="1">
       <c r="B444" s="48" t="s">
@@ -43355,7 +43355,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="446" spans="2:19" ht="36">
+    <row r="446" spans="2:19" ht="48">
       <c r="B446" s="48" t="s">
         <v>1017</v>
       </c>
@@ -43755,7 +43755,7 @@
       </c>
       <c r="S453" s="42"/>
     </row>
-    <row r="454" spans="2:19" ht="14.5">
+    <row r="454" spans="2:19">
       <c r="B454" s="48" t="s">
         <v>1037</v>
       </c>
@@ -43811,7 +43811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="455" spans="2:19" ht="14.5">
+    <row r="455" spans="2:19" ht="24">
       <c r="B455" s="112" t="s">
         <v>1493</v>
       </c>
@@ -43867,7 +43867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="456" spans="2:19" ht="14.5">
+    <row r="456" spans="2:19">
       <c r="B456" s="48" t="s">
         <v>1045</v>
       </c>
@@ -43923,7 +43923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="457" spans="2:19" ht="14.5">
+    <row r="457" spans="2:19" ht="24">
       <c r="B457" s="48" t="s">
         <v>1046</v>
       </c>
@@ -44035,7 +44035,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="459" spans="2:19" ht="14.5">
+    <row r="459" spans="2:19">
       <c r="B459" s="48" t="s">
         <v>1050</v>
       </c>
@@ -44147,7 +44147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="461" spans="2:19" ht="14.5">
+    <row r="461" spans="2:19" ht="24">
       <c r="B461" s="48" t="s">
         <v>1054</v>
       </c>
@@ -44203,7 +44203,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="462" spans="2:19" ht="72">
+    <row r="462" spans="2:19" ht="84">
       <c r="B462" s="48" t="s">
         <v>1057</v>
       </c>
@@ -44255,7 +44255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="463" spans="2:19" ht="60">
+    <row r="463" spans="2:19" ht="72">
       <c r="B463" s="48" t="s">
         <v>1061</v>
       </c>
@@ -44341,7 +44341,7 @@
       </c>
       <c r="S464" s="14"/>
     </row>
-    <row r="465" spans="2:19" ht="36">
+    <row r="465" spans="2:19" ht="48">
       <c r="B465" s="48" t="s">
         <v>1064</v>
       </c>
@@ -44397,7 +44397,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="466" spans="2:19" ht="24">
+    <row r="466" spans="2:19" ht="36">
       <c r="B466" s="48" t="s">
         <v>1066</v>
       </c>
@@ -44561,7 +44561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="469" spans="2:19" ht="60">
+    <row r="469" spans="2:19" ht="84">
       <c r="B469" s="48" t="s">
         <v>1070</v>
       </c>
@@ -44617,7 +44617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="470" spans="2:19" ht="36">
+    <row r="470" spans="2:19" ht="48">
       <c r="B470" s="48" t="s">
         <v>1074</v>
       </c>
@@ -44729,7 +44729,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="472" spans="2:19" ht="120">
+    <row r="472" spans="2:19" ht="144">
       <c r="B472" s="48" t="s">
         <v>1093</v>
       </c>
@@ -44875,7 +44875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="475" spans="2:19" ht="24">
+    <row r="475" spans="2:19" ht="36">
       <c r="B475" s="48" t="s">
         <v>1101</v>
       </c>
@@ -45155,7 +45155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="480" spans="2:19" ht="14.5">
+    <row r="480" spans="2:19" ht="24">
       <c r="B480" s="48" t="s">
         <v>1725</v>
       </c>
@@ -45429,7 +45429,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="485" spans="2:19" ht="14.5">
+    <row r="485" spans="2:19">
       <c r="B485" s="48"/>
       <c r="C485" s="109" t="s">
         <v>1461</v>
@@ -45471,7 +45471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="486" spans="2:19" ht="14.5">
+    <row r="486" spans="2:19">
       <c r="B486" s="48" t="s">
         <v>1111</v>
       </c>
@@ -45527,7 +45527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="487" spans="2:19" ht="14.5">
+    <row r="487" spans="2:19">
       <c r="B487" s="48" t="s">
         <v>1113</v>
       </c>
@@ -45639,7 +45639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="489" spans="2:19" ht="14.5">
+    <row r="489" spans="2:19">
       <c r="B489" s="48" t="s">
         <v>1117</v>
       </c>
@@ -45751,7 +45751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="491" spans="2:19" ht="14.5">
+    <row r="491" spans="2:19">
       <c r="B491" s="48" t="s">
         <v>1121</v>
       </c>
@@ -46235,7 +46235,7 @@
       </c>
       <c r="S499" s="42"/>
     </row>
-    <row r="500" spans="2:19" ht="72" hidden="1">
+    <row r="500" spans="2:19" ht="96" hidden="1">
       <c r="B500" s="48"/>
       <c r="C500" s="109"/>
       <c r="D500" s="110"/>
@@ -46301,7 +46301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="502" spans="2:19" ht="14.5">
+    <row r="502" spans="2:19" ht="24">
       <c r="B502" s="48" t="s">
         <v>1143</v>
       </c>
@@ -46357,7 +46357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="503" spans="2:19" ht="14.5">
+    <row r="503" spans="2:19">
       <c r="B503" s="48" t="s">
         <v>1145</v>
       </c>
@@ -46469,7 +46469,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="505" spans="2:19" ht="24">
+    <row r="505" spans="2:19" ht="36">
       <c r="B505" s="48" t="s">
         <v>1149</v>
       </c>
@@ -46525,7 +46525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="506" spans="2:19" ht="24">
+    <row r="506" spans="2:19" ht="36">
       <c r="B506" s="48" t="s">
         <v>1151</v>
       </c>
@@ -46581,7 +46581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="507" spans="2:19" ht="24">
+    <row r="507" spans="2:19" ht="36">
       <c r="B507" s="48" t="s">
         <v>1157</v>
       </c>
@@ -46749,7 +46749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="510" spans="2:19" ht="36" hidden="1">
+    <row r="510" spans="2:19" ht="48" hidden="1">
       <c r="B510" s="48" t="s">
         <v>1165</v>
       </c>
@@ -46893,7 +46893,7 @@
       </c>
       <c r="S512" s="42"/>
     </row>
-    <row r="513" spans="2:19" ht="36">
+    <row r="513" spans="2:19" ht="48">
       <c r="B513" s="48" t="s">
         <v>1078</v>
       </c>
@@ -46949,7 +46949,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="514" spans="2:19" ht="36">
+    <row r="514" spans="2:19" ht="48">
       <c r="B514" s="48" t="s">
         <v>1080</v>
       </c>
@@ -47005,7 +47005,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="515" spans="2:19" ht="36">
+    <row r="515" spans="2:19" ht="48">
       <c r="B515" s="48" t="s">
         <v>1082</v>
       </c>
@@ -47061,7 +47061,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="516" spans="2:19" ht="36">
+    <row r="516" spans="2:19" ht="48">
       <c r="B516" s="48" t="s">
         <v>1084</v>
       </c>
@@ -47173,7 +47173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="518" spans="2:19" ht="36">
+    <row r="518" spans="2:19" ht="48">
       <c r="B518" s="136" t="s">
         <v>1531</v>
       </c>
@@ -47337,7 +47337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="521" spans="2:19" ht="84" hidden="1">
+    <row r="521" spans="2:19" ht="96" hidden="1">
       <c r="B521" s="136" t="s">
         <v>1533</v>
       </c>
@@ -47387,7 +47387,7 @@
       </c>
       <c r="S521" s="14"/>
     </row>
-    <row r="522" spans="2:19" ht="14.5" hidden="1">
+    <row r="522" spans="2:19" hidden="1">
       <c r="B522" s="88"/>
       <c r="C522" s="106"/>
       <c r="D522" s="110" t="s">
@@ -47423,7 +47423,7 @@
       </c>
       <c r="S522" s="14"/>
     </row>
-    <row r="523" spans="2:19" ht="60" hidden="1">
+    <row r="523" spans="2:19" ht="72" hidden="1">
       <c r="B523" s="48"/>
       <c r="C523" s="106"/>
       <c r="D523" s="107"/>
@@ -47457,7 +47457,7 @@
       </c>
       <c r="S523" s="14"/>
     </row>
-    <row r="524" spans="2:19" ht="72">
+    <row r="524" spans="2:19" ht="84">
       <c r="B524" s="48" t="s">
         <v>1173</v>
       </c>
@@ -47513,7 +47513,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="525" spans="2:19" ht="14.5">
+    <row r="525" spans="2:19">
       <c r="B525" s="48" t="s">
         <v>1179</v>
       </c>
@@ -47569,7 +47569,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="526" spans="2:19" ht="14.5">
+    <row r="526" spans="2:19" ht="24">
       <c r="B526" s="48" t="s">
         <v>1181</v>
       </c>
@@ -47681,7 +47681,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="528" spans="2:19" ht="36">
+    <row r="528" spans="2:19" ht="48">
       <c r="B528" s="48" t="s">
         <v>1186</v>
       </c>
@@ -47737,7 +47737,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="529" spans="2:19" ht="180">
+    <row r="529" spans="2:19" ht="228">
       <c r="B529" s="48" t="s">
         <v>1189</v>
       </c>
@@ -47793,7 +47793,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="530" spans="2:19" ht="48">
+    <row r="530" spans="2:19" ht="60">
       <c r="B530" s="48" t="s">
         <v>1194</v>
       </c>
@@ -47961,7 +47961,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="533" spans="2:19" ht="72">
+    <row r="533" spans="2:19" ht="84">
       <c r="B533" s="112" t="s">
         <v>1496</v>
       </c>
@@ -48017,7 +48017,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="534" spans="2:19" ht="84">
+    <row r="534" spans="2:19" ht="96">
       <c r="B534" s="48" t="s">
         <v>1206</v>
       </c>
@@ -48167,7 +48167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="537" spans="2:19" ht="36">
+    <row r="537" spans="2:19" ht="48">
       <c r="B537" s="48"/>
       <c r="C537" s="109" t="s">
         <v>1461</v>
@@ -48207,7 +48207,7 @@
       </c>
       <c r="S537" s="42"/>
     </row>
-    <row r="538" spans="2:19" ht="108">
+    <row r="538" spans="2:19" ht="120">
       <c r="B538" s="48" t="s">
         <v>1216</v>
       </c>
@@ -48263,7 +48263,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="539" spans="2:19" ht="14.5">
+    <row r="539" spans="2:19">
       <c r="B539" s="48" t="s">
         <v>1228</v>
       </c>
@@ -48319,7 +48319,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="540" spans="2:19" ht="14.5">
+    <row r="540" spans="2:19" ht="24">
       <c r="B540" s="48" t="s">
         <v>1234</v>
       </c>
@@ -48487,7 +48487,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="543" spans="2:19" ht="180">
+    <row r="543" spans="2:19" ht="228">
       <c r="B543" s="48" t="s">
         <v>1252</v>
       </c>
@@ -48543,7 +48543,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="544" spans="2:19" ht="48">
+    <row r="544" spans="2:19" ht="60">
       <c r="B544" s="48" t="s">
         <v>1259</v>
       </c>
@@ -48711,7 +48711,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="547" spans="2:19" ht="72">
+    <row r="547" spans="2:19" ht="84">
       <c r="B547" s="112" t="s">
         <v>1497</v>
       </c>
@@ -48767,7 +48767,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="548" spans="2:19" ht="84">
+    <row r="548" spans="2:19" ht="96">
       <c r="B548" s="48" t="s">
         <v>1281</v>
       </c>
@@ -48877,7 +48877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="550" spans="2:19" ht="14.5">
+    <row r="550" spans="2:19">
       <c r="B550" s="88"/>
       <c r="C550" s="111" t="s">
         <v>1461</v>
@@ -48917,7 +48917,7 @@
       </c>
       <c r="S550" s="42"/>
     </row>
-    <row r="551" spans="2:19" ht="84">
+    <row r="551" spans="2:19" ht="96">
       <c r="B551" s="48" t="s">
         <v>1293</v>
       </c>
@@ -49029,7 +49029,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="553" spans="2:19" ht="72">
+    <row r="553" spans="2:19" ht="84">
       <c r="B553" s="48" t="s">
         <v>1498</v>
       </c>
@@ -49187,7 +49187,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="556" spans="2:19" ht="36">
+    <row r="556" spans="2:19" ht="48">
       <c r="B556" s="112" t="s">
         <v>1316</v>
       </c>
@@ -49243,7 +49243,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="557" spans="2:19" ht="24">
+    <row r="557" spans="2:19" ht="36">
       <c r="B557" s="112"/>
       <c r="C557" s="109" t="s">
         <v>1461</v>
@@ -49353,7 +49353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="559" spans="2:19" ht="24">
+    <row r="559" spans="2:19" ht="36">
       <c r="B559" s="112"/>
       <c r="C559" s="109" t="s">
         <v>1461</v>
@@ -49407,7 +49407,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="560" spans="2:19" ht="24">
+    <row r="560" spans="2:19" ht="36">
       <c r="B560" s="112" t="s">
         <v>1331</v>
       </c>
@@ -49517,7 +49517,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="562" spans="2:19" ht="36">
+    <row r="562" spans="2:19" ht="48">
       <c r="B562" s="112" t="s">
         <v>1336</v>
       </c>
@@ -49627,7 +49627,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="564" spans="2:19" ht="48">
+    <row r="564" spans="2:19" ht="60">
       <c r="B564" s="112" t="s">
         <v>1341</v>
       </c>
@@ -49737,7 +49737,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="566" spans="2:19" ht="144">
+    <row r="566" spans="2:19" ht="156">
       <c r="B566" s="112" t="s">
         <v>1344</v>
       </c>
@@ -49812,16 +49812,16 @@
       <c r="Q567" s="1"/>
     </row>
     <row r="568" spans="2:19" ht="38.25" customHeight="1">
-      <c r="B568" s="197" t="s">
+      <c r="B568" s="226" t="s">
         <v>1350</v>
       </c>
-      <c r="C568" s="197"/>
-      <c r="D568" s="197"/>
-      <c r="E568" s="197"/>
-      <c r="F568" s="197"/>
-      <c r="G568" s="197"/>
-      <c r="H568" s="197"/>
-      <c r="I568" s="197"/>
+      <c r="C568" s="226"/>
+      <c r="D568" s="226"/>
+      <c r="E568" s="226"/>
+      <c r="F568" s="226"/>
+      <c r="G568" s="226"/>
+      <c r="H568" s="226"/>
+      <c r="I568" s="226"/>
       <c r="N568" s="1"/>
       <c r="O568" s="1"/>
       <c r="P568" s="1"/>
@@ -58569,10 +58569,59 @@
       <selection pane="bottomRight" activeCell="A229" sqref="A229"/>
       <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
       <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A5:P528" xr:uid="{41FFD555-4B71-4142-9290-A027F5D28BAB}"/>
+      <autoFilter ref="A5:P528" xr:uid="{252CF8F9-1D13-4D2E-8C51-F87E422AA72C}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="65">
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="R442:R443"/>
+    <mergeCell ref="S442:S443"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="B568:I568"/>
+    <mergeCell ref="B16:B31"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C16:E31"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="P442:P443"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="B570:I570"/>
+    <mergeCell ref="C353:E353"/>
+    <mergeCell ref="C429:E429"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="C285:E285"/>
+    <mergeCell ref="C343:E343"/>
+    <mergeCell ref="C225:C226"/>
+    <mergeCell ref="D225:D226"/>
+    <mergeCell ref="E225:E226"/>
+    <mergeCell ref="Q442:Q443"/>
+    <mergeCell ref="N442:N443"/>
+    <mergeCell ref="O442:O443"/>
+    <mergeCell ref="P225:P226"/>
+    <mergeCell ref="J225:J226"/>
+    <mergeCell ref="K225:K226"/>
+    <mergeCell ref="L225:L226"/>
+    <mergeCell ref="M225:M226"/>
+    <mergeCell ref="J442:J443"/>
+    <mergeCell ref="K442:K443"/>
+    <mergeCell ref="L442:L443"/>
+    <mergeCell ref="M442:M443"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="R225:R226"/>
     <mergeCell ref="S225:S226"/>
@@ -58589,55 +58638,6 @@
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q442:Q443"/>
-    <mergeCell ref="N442:N443"/>
-    <mergeCell ref="O442:O443"/>
-    <mergeCell ref="P225:P226"/>
-    <mergeCell ref="J225:J226"/>
-    <mergeCell ref="K225:K226"/>
-    <mergeCell ref="L225:L226"/>
-    <mergeCell ref="M225:M226"/>
-    <mergeCell ref="J442:J443"/>
-    <mergeCell ref="K442:K443"/>
-    <mergeCell ref="L442:L443"/>
-    <mergeCell ref="M442:M443"/>
-    <mergeCell ref="B570:I570"/>
-    <mergeCell ref="C353:E353"/>
-    <mergeCell ref="C429:E429"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="C285:E285"/>
-    <mergeCell ref="C343:E343"/>
-    <mergeCell ref="C225:C226"/>
-    <mergeCell ref="D225:D226"/>
-    <mergeCell ref="E225:E226"/>
-    <mergeCell ref="R442:R443"/>
-    <mergeCell ref="S442:S443"/>
-    <mergeCell ref="B225:B226"/>
-    <mergeCell ref="B568:I568"/>
-    <mergeCell ref="B16:B31"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C16:E31"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="P442:P443"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:C4 C5:E5 B6:C6 N7:O10 B8:E12 F12:S12 C14:E14 B15:E15 N15:O30 F15:M72 B16:C16 N32:O72 B47:C47 B48:E60 C48:E72 B62:E72 P68:Q72 B73:Q76 B77:S78 B79:O93 P91:S93 N94:S99 F94:M113 B94:E139 N100:O113 B141:O143 N144:O147 B144:E183 F144:M197 N167:O197 B179:M181 B184:C184 B194:E197 P194:Q201 B198:O200 J201:O201 P213:Q214 B213:O225 B227:O284 Q239:Q245 P246:Q255 Q256:Q259 P256:P283 Q261:Q283 P284:Q371 B285:C285 F285:O285 B286:O318 B319:M342 N319:O371 B343:C343 F343:M343 B344:M352 B353:C353 F353:M353 B354:M394 T370:T371 N372:Q394 B395:Q395 N396:Q422 B396:M428 O423 Q423 N424:O437 B429:C429 F429:M429 B430:M437 B443:I443 N443:O443 B444:O470 P448:P467 Q449:Q467 L468:Q468 P470:Q470 B471:Q510">
     <cfRule type="expression" dxfId="201" priority="17677">
@@ -59455,6 +59455,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c7d0ed18-d4ec-4450-b043-97ba750af715"/>
+    <_dlc_DocId xmlns="053a5afd-1424-405b-82d9-63deec7446f8">DZXA3YQD6WY2-1198327409-85</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="053a5afd-1424-405b-82d9-63deec7446f8">
+      <Url>https://sharepoint.hrsa.gov/teams/mchb/oer/nsch/_layouts/15/DocIdRedir.aspx?ID=DZXA3YQD6WY2-1198327409-85</Url>
+      <Description>DZXA3YQD6WY2-1198327409-85</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -59502,28 +59524,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c7d0ed18-d4ec-4450-b043-97ba750af715"/>
-    <_dlc_DocId xmlns="053a5afd-1424-405b-82d9-63deec7446f8">DZXA3YQD6WY2-1198327409-85</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="053a5afd-1424-405b-82d9-63deec7446f8">
-      <Url>https://sharepoint.hrsa.gov/teams/mchb/oer/nsch/_layouts/15/DocIdRedir.aspx?ID=DZXA3YQD6WY2-1198327409-85</Url>
-      <Description>DZXA3YQD6WY2-1198327409-85</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59701,9 +59701,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27AEA45-1C93-4ED8-836C-379A7FF37C5F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{698216AE-EB17-4A50-AF0E-2A1D4A5A12B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="053a5afd-1424-405b-82d9-63deec7446f8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c7d0ed18-d4ec-4450-b043-97ba750af715"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -59717,18 +59726,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{698216AE-EB17-4A50-AF0E-2A1D4A5A12B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27AEA45-1C93-4ED8-836C-379A7FF37C5F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="053a5afd-1424-405b-82d9-63deec7446f8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c7d0ed18-d4ec-4450-b043-97ba750af715"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>